<commit_message>
Ax 15H int refund -- Chkd Tax status: OK
</commit_message>
<xml_diff>
--- a/Fix/fix cur. 15.xlsx
+++ b/Fix/fix cur. 15.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="43">
   <si>
     <t>amt</t>
   </si>
@@ -137,9 +137,6 @@
   </si>
   <si>
     <t>16+11</t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
   <si>
     <t xml:space="preserve">24106000093949  </t>
@@ -780,7 +777,7 @@
   <dimension ref="A1:U106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1032,9 +1029,7 @@
       <c r="E7" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="48" t="s">
-        <v>41</v>
-      </c>
+      <c r="F7" s="48"/>
       <c r="G7" s="49">
         <v>41223</v>
       </c>
@@ -1123,7 +1118,7 @@
       <c r="H9" s="28">
         <v>42210</v>
       </c>
-      <c r="I9" s="54">
+      <c r="I9" s="44">
         <v>4830</v>
       </c>
       <c r="J9" s="32" t="s">
@@ -1319,7 +1314,7 @@
         <v>10125</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="11"/>
@@ -1829,7 +1824,7 @@
         <v>375</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K27" s="3"/>
       <c r="L27" s="4"/>

</xml_diff>